<commit_message>
For comparing the two studies
Panetsos data for North Bay and East bay will bo compared with my North Bay data.
</commit_message>
<xml_diff>
--- a/Radish_data/Radish1.xlsx
+++ b/Radish_data/Radish1.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32d330a05a62be0e/Science/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32d330a05a62be0e/Documents/GitHub/Miscellanea_Pythonica/Radish_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{DDBA9C7C-2A7D-45B3-8D67-EA3EA9753F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A492C85C-D3CF-4226-B6BC-162527B88CD2}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{DDBA9C7C-2A7D-45B3-8D67-EA3EA9753F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5EF31CC-2BCE-4F2A-8589-913741160976}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{AA3D5D6E-8EB8-4971-9089-662C6FD956D6}"/>
+    <workbookView xWindow="72" yWindow="288" windowWidth="16560" windowHeight="10884" firstSheet="1" activeTab="1" xr2:uid="{AA3D5D6E-8EB8-4971-9089-662C6FD956D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Panetsos" sheetId="1" r:id="rId1"/>
-    <sheet name="By_Hab" sheetId="2" r:id="rId2"/>
-    <sheet name="By_Loc" sheetId="3" r:id="rId3"/>
-    <sheet name="Loc_groups" sheetId="4" r:id="rId4"/>
-    <sheet name="Hab_groups" sheetId="5" r:id="rId5"/>
+    <sheet name="Now_vs_Then" sheetId="6" r:id="rId2"/>
+    <sheet name="By_Hab" sheetId="2" r:id="rId3"/>
+    <sheet name="By_Loc" sheetId="3" r:id="rId4"/>
+    <sheet name="Loc_groups" sheetId="4" r:id="rId5"/>
+    <sheet name="Hab_groups" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029" iterate="1"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId6"/>
     <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="74">
   <si>
     <t>S. Delta</t>
   </si>
@@ -218,6 +219,51 @@
   </si>
   <si>
     <t>By</t>
+  </si>
+  <si>
+    <t>Locality</t>
+  </si>
+  <si>
+    <t>Lake Dalwigk</t>
+  </si>
+  <si>
+    <t>White Slough</t>
+  </si>
+  <si>
+    <t>American Canyon</t>
+  </si>
+  <si>
+    <t>Napa Valley College</t>
+  </si>
+  <si>
+    <t>West Napa</t>
+  </si>
+  <si>
+    <t>Congress Valley</t>
+  </si>
+  <si>
+    <t>Mare Island</t>
+  </si>
+  <si>
+    <t>Coombsville</t>
+  </si>
+  <si>
+    <t>Suscol Creek</t>
+  </si>
+  <si>
+    <t>Panetsos Vallejo</t>
+  </si>
+  <si>
+    <t>Panetsos Petaluma</t>
+  </si>
+  <si>
+    <t>Panetsos El Cerrito</t>
+  </si>
+  <si>
+    <t>Panetsos Berkeley</t>
+  </si>
+  <si>
+    <t>Panetsos Holy Names</t>
   </si>
 </sst>
 </file>
@@ -275,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -291,15 +337,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -834,7 +881,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BFA957E7-19E8-4F1F-9AAA-719444294BBD}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BFA957E7-19E8-4F1F-9AAA-719444294BBD}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G2:J7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -904,7 +951,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E204914F-5B1F-43D7-A8EE-C7ADE5CADC09}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E204914F-5B1F-43D7-A8EE-C7ADE5CADC09}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H3:K11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -1359,6 +1406,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
@@ -1427,23 +1477,23 @@
         <v>2</v>
       </c>
       <c r="I2">
-        <f>SUM(E2:H2)</f>
+        <f t="shared" ref="I2:I29" si="0">SUM(E2:H2)</f>
         <v>100</v>
       </c>
       <c r="J2" s="1">
-        <f>E2/I2</f>
+        <f t="shared" ref="J2:J29" si="1">E2/I2</f>
         <v>0.78</v>
       </c>
       <c r="K2" s="1">
-        <f>F2/I2</f>
+        <f t="shared" ref="K2:K29" si="2">F2/I2</f>
         <v>0.02</v>
       </c>
       <c r="L2" s="1">
-        <f>G2/I2</f>
+        <f t="shared" ref="L2:L29" si="3">G2/I2</f>
         <v>0.18</v>
       </c>
       <c r="M2" s="1">
-        <f>H2/I2</f>
+        <f t="shared" ref="M2:M29" si="4">H2/I2</f>
         <v>0.02</v>
       </c>
     </row>
@@ -1473,23 +1523,23 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <f>SUM(E3:H3)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J3" s="1">
-        <f>E3/I3</f>
+        <f t="shared" si="1"/>
         <v>0.78</v>
       </c>
       <c r="K3" s="1">
-        <f>F3/I3</f>
+        <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
       <c r="L3" s="1">
-        <f>G3/I3</f>
+        <f t="shared" si="3"/>
         <v>0.19</v>
       </c>
       <c r="M3" s="1">
-        <f>H3/I3</f>
+        <f t="shared" si="4"/>
         <v>0.01</v>
       </c>
     </row>
@@ -1519,23 +1569,23 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <f>SUM(E4:H4)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J4" s="1">
-        <f>E4/I4</f>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="K4" s="1">
-        <f>F4/I4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L4" s="1">
-        <f>G4/I4</f>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="M4" s="1">
-        <f>H4/I4</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1565,23 +1615,23 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <f>SUM(E5:H5)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J5" s="1">
-        <f>E5/I5</f>
+        <f t="shared" si="1"/>
         <v>0.62</v>
       </c>
       <c r="K5" s="1">
-        <f>F5/I5</f>
+        <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
       <c r="L5" s="1">
-        <f>G5/I5</f>
+        <f t="shared" si="3"/>
         <v>0.32</v>
       </c>
       <c r="M5" s="1">
-        <f>H5/I5</f>
+        <f t="shared" si="4"/>
         <v>0.01</v>
       </c>
     </row>
@@ -1611,23 +1661,23 @@
         <v>0.8</v>
       </c>
       <c r="I6">
-        <f>SUM(E6:H6)</f>
+        <f t="shared" si="0"/>
         <v>100.2</v>
       </c>
       <c r="J6" s="1">
-        <f>E6/I6</f>
+        <f t="shared" si="1"/>
         <v>0.84830339321357284</v>
       </c>
       <c r="K6" s="1">
-        <f>F6/I6</f>
+        <f t="shared" si="2"/>
         <v>3.9920159680638728E-3</v>
       </c>
       <c r="L6" s="1">
-        <f>G6/I6</f>
+        <f t="shared" si="3"/>
         <v>0.13972055888223553</v>
       </c>
       <c r="M6" s="1">
-        <f>H6/I6</f>
+        <f t="shared" si="4"/>
         <v>7.9840319361277456E-3</v>
       </c>
     </row>
@@ -1657,23 +1707,23 @@
         <v>2</v>
       </c>
       <c r="I7">
-        <f>SUM(E7:H7)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J7" s="1">
-        <f>E7/I7</f>
+        <f t="shared" si="1"/>
         <v>0.33</v>
       </c>
       <c r="K7" s="1">
-        <f>F7/I7</f>
+        <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
       <c r="L7" s="1">
-        <f>G7/I7</f>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="M7" s="1">
-        <f>H7/I7</f>
+        <f t="shared" si="4"/>
         <v>0.02</v>
       </c>
     </row>
@@ -1703,23 +1753,23 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <f>SUM(E8:H8)</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="J8" s="1">
-        <f>E8/I8</f>
+        <f t="shared" si="1"/>
         <v>0.82105263157894737</v>
       </c>
       <c r="K8" s="1">
-        <f>F8/I8</f>
+        <f t="shared" si="2"/>
         <v>3.1578947368421054E-2</v>
       </c>
       <c r="L8" s="1">
-        <f>G8/I8</f>
+        <f t="shared" si="3"/>
         <v>0.14736842105263157</v>
       </c>
       <c r="M8" s="1">
-        <f>H8/I8</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1749,23 +1799,23 @@
         <v>3</v>
       </c>
       <c r="I9">
-        <f>SUM(E9:H9)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J9" s="1">
-        <f>E9/I9</f>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="K9" s="1">
-        <f>F9/I9</f>
+        <f t="shared" si="2"/>
         <v>0.22</v>
       </c>
       <c r="L9" s="1">
-        <f>G9/I9</f>
+        <f t="shared" si="3"/>
         <v>0.35</v>
       </c>
       <c r="M9" s="1">
-        <f>H9/I9</f>
+        <f t="shared" si="4"/>
         <v>0.03</v>
       </c>
     </row>
@@ -1795,23 +1845,23 @@
         <v>4</v>
       </c>
       <c r="I10">
-        <f>SUM(E10:H10)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J10" s="1">
-        <f>E10/I10</f>
+        <f t="shared" si="1"/>
         <v>0.47</v>
       </c>
       <c r="K10" s="1">
-        <f>F10/I10</f>
+        <f t="shared" si="2"/>
         <v>0.13</v>
       </c>
       <c r="L10" s="1">
-        <f>G10/I10</f>
+        <f t="shared" si="3"/>
         <v>0.36</v>
       </c>
       <c r="M10" s="1">
-        <f>H10/I10</f>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
     </row>
@@ -1841,23 +1891,23 @@
         <v>2</v>
       </c>
       <c r="I11">
-        <f>SUM(E11:H11)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J11" s="1">
-        <f>E11/I11</f>
+        <f t="shared" si="1"/>
         <v>0.32</v>
       </c>
       <c r="K11" s="1">
-        <f>F11/I11</f>
+        <f t="shared" si="2"/>
         <v>0.16</v>
       </c>
       <c r="L11" s="1">
-        <f>G11/I11</f>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="M11" s="1">
-        <f>H11/I11</f>
+        <f t="shared" si="4"/>
         <v>0.02</v>
       </c>
     </row>
@@ -1887,23 +1937,23 @@
         <v>2</v>
       </c>
       <c r="I12" s="3">
-        <f>SUM(E12:H12)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J12" s="2">
-        <f>E12/I12</f>
+        <f t="shared" si="1"/>
         <v>0.62</v>
       </c>
       <c r="K12" s="2">
-        <f>F12/I12</f>
+        <f t="shared" si="2"/>
         <v>0.16</v>
       </c>
       <c r="L12" s="2">
-        <f>G12/I12</f>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="M12" s="2">
-        <f>H12/I12</f>
+        <f t="shared" si="4"/>
         <v>0.02</v>
       </c>
     </row>
@@ -1933,23 +1983,23 @@
         <v>3</v>
       </c>
       <c r="I13">
-        <f>SUM(E13:H13)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J13" s="1">
-        <f>E13/I13</f>
+        <f t="shared" si="1"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="K13" s="1">
-        <f>F13/I13</f>
+        <f t="shared" si="2"/>
         <v>0.72</v>
       </c>
       <c r="L13" s="1">
-        <f>G13/I13</f>
+        <f t="shared" si="3"/>
         <v>0.11</v>
       </c>
       <c r="M13" s="1">
-        <f>H13/I13</f>
+        <f t="shared" si="4"/>
         <v>0.03</v>
       </c>
     </row>
@@ -1979,23 +2029,23 @@
         <v>3</v>
       </c>
       <c r="I14">
-        <f>SUM(E14:H14)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J14" s="1">
-        <f>E14/I14</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="K14" s="1">
-        <f>F14/I14</f>
+        <f t="shared" si="2"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="L14" s="1">
-        <f>G14/I14</f>
+        <f t="shared" si="3"/>
         <v>0.32</v>
       </c>
       <c r="M14" s="1">
-        <f>H14/I14</f>
+        <f t="shared" si="4"/>
         <v>0.03</v>
       </c>
     </row>
@@ -2025,23 +2075,23 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <f>SUM(E15:H15)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J15" s="1">
-        <f>E15/I15</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K15" s="1">
-        <f>F15/I15</f>
+        <f t="shared" si="2"/>
         <v>0.93</v>
       </c>
       <c r="L15" s="1">
-        <f>G15/I15</f>
+        <f t="shared" si="3"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="M15" s="1">
-        <f>H15/I15</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2071,23 +2121,23 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <f>SUM(E16:H16)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J16" s="1">
-        <f>E16/I16</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K16" s="1">
-        <f>F16/I16</f>
+        <f t="shared" si="2"/>
         <v>0.85</v>
       </c>
       <c r="L16" s="1">
-        <f>G16/I16</f>
+        <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
       <c r="M16" s="1">
-        <f>H16/I16</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2117,23 +2167,23 @@
         <v>2</v>
       </c>
       <c r="I17">
-        <f>SUM(E17:H17)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J17" s="1">
-        <f>E17/I17</f>
+        <f t="shared" si="1"/>
         <v>0.08</v>
       </c>
       <c r="K17" s="1">
-        <f>F17/I17</f>
+        <f t="shared" si="2"/>
         <v>0.52</v>
       </c>
       <c r="L17" s="1">
-        <f>G17/I17</f>
+        <f t="shared" si="3"/>
         <v>0.38</v>
       </c>
       <c r="M17" s="1">
-        <f>H17/I17</f>
+        <f t="shared" si="4"/>
         <v>0.02</v>
       </c>
     </row>
@@ -2163,23 +2213,23 @@
         <v>2</v>
       </c>
       <c r="I18">
-        <f>SUM(E18:H18)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J18" s="1">
-        <f>E18/I18</f>
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
       <c r="K18" s="1">
-        <f>F18/I18</f>
+        <f t="shared" si="2"/>
         <v>0.64</v>
       </c>
       <c r="L18" s="1">
-        <f>G18/I18</f>
+        <f t="shared" si="3"/>
         <v>0.31</v>
       </c>
       <c r="M18" s="1">
-        <f>H18/I18</f>
+        <f t="shared" si="4"/>
         <v>0.02</v>
       </c>
     </row>
@@ -2209,23 +2259,23 @@
         <v>1</v>
       </c>
       <c r="I19">
-        <f>SUM(E19:H19)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J19" s="1">
-        <f>E19/I19</f>
+        <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
       <c r="K19" s="1">
-        <f>F19/I19</f>
+        <f t="shared" si="2"/>
         <v>0.32</v>
       </c>
       <c r="L19" s="1">
-        <f>G19/I19</f>
+        <f t="shared" si="3"/>
         <v>0.49</v>
       </c>
       <c r="M19" s="1">
-        <f>H19/I19</f>
+        <f t="shared" si="4"/>
         <v>0.01</v>
       </c>
     </row>
@@ -2255,23 +2305,23 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <f>SUM(E20:H20)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J20" s="1">
-        <f>E20/I20</f>
+        <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
       <c r="K20" s="1">
-        <f>F20/I20</f>
+        <f t="shared" si="2"/>
         <v>0.32</v>
       </c>
       <c r="L20" s="1">
-        <f>G20/I20</f>
+        <f t="shared" si="3"/>
         <v>0.49</v>
       </c>
       <c r="M20" s="1">
-        <f>H20/I20</f>
+        <f t="shared" si="4"/>
         <v>0.01</v>
       </c>
     </row>
@@ -2301,23 +2351,23 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <f>SUM(E21:H21)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J21" s="1">
-        <f>E21/I21</f>
+        <f t="shared" si="1"/>
         <v>0.89</v>
       </c>
       <c r="K21" s="1">
-        <f>F21/I21</f>
+        <f t="shared" si="2"/>
         <v>0.06</v>
       </c>
       <c r="L21" s="1">
-        <f>G21/I21</f>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="M21" s="1">
-        <f>H21/I21</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2347,23 +2397,23 @@
         <v>4</v>
       </c>
       <c r="I22">
-        <f>SUM(E22:H22)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J22" s="1">
-        <f>E22/I22</f>
+        <f t="shared" si="1"/>
         <v>0.71</v>
       </c>
       <c r="K22" s="1">
-        <f>F22/I22</f>
+        <f t="shared" si="2"/>
         <v>0.04</v>
       </c>
       <c r="L22" s="1">
-        <f>G22/I22</f>
+        <f t="shared" si="3"/>
         <v>0.21</v>
       </c>
       <c r="M22" s="1">
-        <f>H22/I22</f>
+        <f t="shared" si="4"/>
         <v>0.04</v>
       </c>
     </row>
@@ -2393,23 +2443,23 @@
         <v>11</v>
       </c>
       <c r="I23">
-        <f>SUM(E23:H23)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J23" s="1">
-        <f>E23/I23</f>
+        <f t="shared" si="1"/>
         <v>0.78</v>
       </c>
       <c r="K23" s="1">
-        <f>F23/I23</f>
+        <f t="shared" si="2"/>
         <v>0.03</v>
       </c>
       <c r="L23" s="1">
-        <f>G23/I23</f>
+        <f t="shared" si="3"/>
         <v>0.08</v>
       </c>
       <c r="M23" s="1">
-        <f>H23/I23</f>
+        <f t="shared" si="4"/>
         <v>0.11</v>
       </c>
     </row>
@@ -2439,23 +2489,23 @@
         <v>4</v>
       </c>
       <c r="I24">
-        <f>SUM(E24:H24)</f>
+        <f t="shared" si="0"/>
         <v>101</v>
       </c>
       <c r="J24" s="1">
-        <f>E24/I24</f>
+        <f t="shared" si="1"/>
         <v>0.11881188118811881</v>
       </c>
       <c r="K24" s="1">
-        <f>F24/I24</f>
+        <f t="shared" si="2"/>
         <v>0.47524752475247523</v>
       </c>
       <c r="L24" s="1">
-        <f>G24/I24</f>
+        <f t="shared" si="3"/>
         <v>0.36633663366336633</v>
       </c>
       <c r="M24" s="1">
-        <f>H24/I24</f>
+        <f t="shared" si="4"/>
         <v>3.9603960396039604E-2</v>
       </c>
     </row>
@@ -2485,23 +2535,23 @@
         <v>6</v>
       </c>
       <c r="I25">
-        <f>SUM(E25:H25)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J25" s="1">
-        <f>E25/I25</f>
+        <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
       <c r="K25" s="1">
-        <f>F25/I25</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="L25" s="1">
-        <f>G25/I25</f>
+        <f t="shared" si="3"/>
         <v>0.32</v>
       </c>
       <c r="M25" s="1">
-        <f>H25/I25</f>
+        <f t="shared" si="4"/>
         <v>0.06</v>
       </c>
     </row>
@@ -2531,23 +2581,23 @@
         <v>4</v>
       </c>
       <c r="I26">
-        <f>SUM(E26:H26)</f>
+        <f t="shared" si="0"/>
         <v>101</v>
       </c>
       <c r="J26" s="1">
-        <f>E26/I26</f>
+        <f t="shared" si="1"/>
         <v>0.29702970297029702</v>
       </c>
       <c r="K26" s="1">
-        <f>F26/I26</f>
+        <f t="shared" si="2"/>
         <v>8.9108910891089105E-2</v>
       </c>
       <c r="L26" s="1">
-        <f>G26/I26</f>
+        <f t="shared" si="3"/>
         <v>0.57425742574257421</v>
       </c>
       <c r="M26" s="1">
-        <f>H26/I26</f>
+        <f t="shared" si="4"/>
         <v>3.9603960396039604E-2</v>
       </c>
     </row>
@@ -2577,23 +2627,23 @@
         <v>7</v>
       </c>
       <c r="I27">
-        <f>SUM(E27:H27)</f>
+        <f t="shared" si="0"/>
         <v>101</v>
       </c>
       <c r="J27" s="1">
-        <f>E27/I27</f>
+        <f t="shared" si="1"/>
         <v>0.38613861386138615</v>
       </c>
       <c r="K27" s="1">
-        <f>F27/I27</f>
+        <f t="shared" si="2"/>
         <v>0.14851485148514851</v>
       </c>
       <c r="L27" s="1">
-        <f>G27/I27</f>
+        <f t="shared" si="3"/>
         <v>0.39603960396039606</v>
       </c>
       <c r="M27" s="1">
-        <f>H27/I27</f>
+        <f t="shared" si="4"/>
         <v>6.9306930693069313E-2</v>
       </c>
     </row>
@@ -2623,23 +2673,23 @@
         <v>3</v>
       </c>
       <c r="I28">
-        <f>SUM(E28:H28)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J28" s="1">
-        <f>E28/I28</f>
+        <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
       <c r="K28" s="1">
-        <f>F28/I28</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="L28" s="1">
-        <f>G28/I28</f>
+        <f t="shared" si="3"/>
         <v>0.48</v>
       </c>
       <c r="M28" s="1">
-        <f>H28/I28</f>
+        <f t="shared" si="4"/>
         <v>0.03</v>
       </c>
     </row>
@@ -2669,23 +2719,23 @@
         <v>6</v>
       </c>
       <c r="I29">
-        <f>SUM(E29:H29)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J29" s="1">
-        <f>E29/I29</f>
+        <f t="shared" si="1"/>
         <v>0.13</v>
       </c>
       <c r="K29" s="1">
-        <f>F29/I29</f>
+        <f t="shared" si="2"/>
         <v>0.54</v>
       </c>
       <c r="L29" s="1">
-        <f>G29/I29</f>
+        <f t="shared" si="3"/>
         <v>0.27</v>
       </c>
       <c r="M29" s="1">
-        <f>H29/I29</f>
+        <f t="shared" si="4"/>
         <v>0.06</v>
       </c>
     </row>
@@ -2695,6 +2745,235 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9904AB-0918-46EF-A98E-60B70B497290}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="12">
+        <v>0.5988</v>
+      </c>
+      <c r="C2" s="12">
+        <v>6.6E-3</v>
+      </c>
+      <c r="D2" s="12">
+        <v>2.29E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="12">
+        <v>0.71089999999999998</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="D3" s="12">
+        <v>3.0599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.66720000000000002</v>
+      </c>
+      <c r="C4">
+        <v>2.83</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="12">
+        <v>0.64580000000000004</v>
+      </c>
+      <c r="C5" s="12">
+        <v>3.2099999999999997E-2</v>
+      </c>
+      <c r="D5" s="12">
+        <v>5.1400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.85</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0.88890000000000002</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0.63180000000000003</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0</v>
+      </c>
+      <c r="D8" s="12">
+        <v>1.9900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="12">
+        <v>0.31259999999999999</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.15379999999999999</v>
+      </c>
+      <c r="D10" s="12">
+        <v>7.3400000000000007E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="12">
+        <v>0.62</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0.16</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0.72</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="12">
+        <v>0.32</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0.16</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="12">
+        <v>0.47</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.13</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.22</v>
+      </c>
+      <c r="D15" s="12">
+        <v>0.03</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147FD0A7-316F-4E56-A584-86898D60136E}">
   <dimension ref="A1:N30"/>
   <sheetViews>
@@ -2736,7 +3015,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <f>SUM(B2:D2)</f>
+        <f t="shared" ref="E2:E29" si="0">SUM(B2:D2)</f>
         <v>80</v>
       </c>
       <c r="G2" s="6" t="s">
@@ -2766,7 +3045,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <f>SUM(B3:D3)</f>
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -2796,7 +3075,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <f>SUM(B4:D4)</f>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
       <c r="G4" s="5" t="s">
@@ -2826,7 +3105,7 @@
         <v>2</v>
       </c>
       <c r="E5">
-        <f>SUM(B5:D5)</f>
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -2856,7 +3135,7 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <f>SUM(B6:D6)</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="G6" s="5" t="s">
@@ -2886,7 +3165,7 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <f>SUM(B7:D7)</f>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="G7" s="5" t="s">
@@ -2916,7 +3195,7 @@
         <v>3</v>
       </c>
       <c r="E8">
-        <f>SUM(B8:D8)</f>
+        <f t="shared" si="0"/>
         <v>89</v>
       </c>
     </row>
@@ -2934,7 +3213,7 @@
         <v>4</v>
       </c>
       <c r="E9">
-        <f>SUM(B9:D9)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
@@ -2952,7 +3231,7 @@
         <v>0.8</v>
       </c>
       <c r="E10">
-        <f>SUM(B10:D10)</f>
+        <f t="shared" si="0"/>
         <v>86.2</v>
       </c>
     </row>
@@ -2970,7 +3249,7 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <f>SUM(B11:D11)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
     </row>
@@ -2988,7 +3267,7 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <f>SUM(B12:D12)</f>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
     </row>
@@ -3006,7 +3285,7 @@
         <v>2</v>
       </c>
       <c r="E13">
-        <f>SUM(B13:D13)</f>
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="N13" t="s">
@@ -3027,7 +3306,7 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <f>SUM(B14:D14)</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
     </row>
@@ -3045,7 +3324,7 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <f>SUM(B15:D15)</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
     </row>
@@ -3063,7 +3342,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <f>SUM(B16:D16)</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
     </row>
@@ -3081,7 +3360,7 @@
         <v>4</v>
       </c>
       <c r="E17">
-        <f>SUM(B17:D17)</f>
+        <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
@@ -3099,7 +3378,7 @@
         <v>11</v>
       </c>
       <c r="E18">
-        <f>SUM(B18:D18)</f>
+        <f t="shared" si="0"/>
         <v>92</v>
       </c>
     </row>
@@ -3117,7 +3396,7 @@
         <v>4</v>
       </c>
       <c r="E19">
-        <f>SUM(B19:D19)</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
@@ -3135,7 +3414,7 @@
         <v>6</v>
       </c>
       <c r="E20">
-        <f>SUM(B20:D20)</f>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
     </row>
@@ -3153,7 +3432,7 @@
         <v>7</v>
       </c>
       <c r="E21">
-        <f>SUM(B21:D21)</f>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
     </row>
@@ -3171,7 +3450,7 @@
         <v>3</v>
       </c>
       <c r="E22">
-        <f>SUM(B22:D22)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
@@ -3189,7 +3468,7 @@
         <v>6</v>
       </c>
       <c r="E23">
-        <f>SUM(B23:D23)</f>
+        <f t="shared" si="0"/>
         <v>73</v>
       </c>
     </row>
@@ -3207,7 +3486,7 @@
         <v>2</v>
       </c>
       <c r="E24">
-        <f>SUM(B24:D24)</f>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
     </row>
@@ -3225,7 +3504,7 @@
         <v>2</v>
       </c>
       <c r="E25">
-        <f>SUM(B25:D25)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
@@ -3243,7 +3522,7 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <f>SUM(B26:D26)</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
     </row>
@@ -3261,7 +3540,7 @@
         <v>3</v>
       </c>
       <c r="E27">
-        <f>SUM(B27:D27)</f>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
     </row>
@@ -3279,7 +3558,7 @@
         <v>4</v>
       </c>
       <c r="E28">
-        <f>SUM(B28:D28)</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
@@ -3297,7 +3576,7 @@
         <v>2</v>
       </c>
       <c r="E29">
-        <f>SUM(B29:D29)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
@@ -3323,7 +3602,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80121CBB-3591-48EF-BFEA-FA467836A32B}">
   <dimension ref="A1:K30"/>
   <sheetViews>
@@ -3365,7 +3644,7 @@
         <v>3</v>
       </c>
       <c r="E2">
-        <f>SUM(B2:D2)</f>
+        <f t="shared" ref="E2:E29" si="0">SUM(B2:D2)</f>
         <v>68</v>
       </c>
     </row>
@@ -3383,7 +3662,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <f>SUM(B3:D3)</f>
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
       <c r="H3" s="6" t="s">
@@ -3413,7 +3692,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <f>SUM(B4:D4)</f>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
       <c r="H4" s="5" t="s">
@@ -3443,7 +3722,7 @@
         <v>2</v>
       </c>
       <c r="E5">
-        <f>SUM(B5:D5)</f>
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -3473,7 +3752,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <f>SUM(B6:D6)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="H6" s="5" t="s">
@@ -3503,7 +3782,7 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <f>SUM(B7:D7)</f>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="H7" s="5" t="s">
@@ -3533,7 +3812,7 @@
         <v>0.8</v>
       </c>
       <c r="E8">
-        <f>SUM(B8:D8)</f>
+        <f t="shared" si="0"/>
         <v>86.2</v>
       </c>
       <c r="H8" s="5" t="s">
@@ -3563,7 +3842,7 @@
         <v>2</v>
       </c>
       <c r="E9">
-        <f>SUM(B9:D9)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="H9" s="5" t="s">
@@ -3593,7 +3872,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <f>SUM(B10:D10)</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="H10" s="5" t="s">
@@ -3623,7 +3902,7 @@
         <v>4</v>
       </c>
       <c r="E11">
-        <f>SUM(B11:D11)</f>
+        <f t="shared" si="0"/>
         <v>79</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -3653,7 +3932,7 @@
         <v>11</v>
       </c>
       <c r="E12">
-        <f>SUM(B12:D12)</f>
+        <f t="shared" si="0"/>
         <v>92</v>
       </c>
     </row>
@@ -3671,7 +3950,7 @@
         <v>3</v>
       </c>
       <c r="E13">
-        <f>SUM(B13:D13)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
@@ -3689,7 +3968,7 @@
         <v>6</v>
       </c>
       <c r="E14">
-        <f>SUM(B14:D14)</f>
+        <f t="shared" si="0"/>
         <v>73</v>
       </c>
     </row>
@@ -3707,7 +3986,7 @@
         <v>2</v>
       </c>
       <c r="E15">
-        <f>SUM(B15:D15)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
     </row>
@@ -3725,7 +4004,7 @@
         <v>3</v>
       </c>
       <c r="E16">
-        <f>SUM(B16:D16)</f>
+        <f t="shared" si="0"/>
         <v>89</v>
       </c>
     </row>
@@ -3743,7 +4022,7 @@
         <v>2</v>
       </c>
       <c r="E17">
-        <f>SUM(B17:D17)</f>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
     </row>
@@ -3761,7 +4040,7 @@
         <v>1</v>
       </c>
       <c r="E18">
-        <f>SUM(B18:D18)</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
     </row>
@@ -3779,7 +4058,7 @@
         <v>4</v>
       </c>
       <c r="E19">
-        <f>SUM(B19:D19)</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
@@ -3797,7 +4076,7 @@
         <v>3</v>
       </c>
       <c r="E20">
-        <f>SUM(B20:D20)</f>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
     </row>
@@ -3815,7 +4094,7 @@
         <v>4</v>
       </c>
       <c r="E21">
-        <f>SUM(B21:D21)</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
@@ -3833,7 +4112,7 @@
         <v>2</v>
       </c>
       <c r="E22">
-        <f>SUM(B22:D22)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
@@ -3851,7 +4130,7 @@
         <v>6</v>
       </c>
       <c r="E23">
-        <f>SUM(B23:D23)</f>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
     </row>
@@ -3869,7 +4148,7 @@
         <v>4</v>
       </c>
       <c r="E24">
-        <f>SUM(B24:D24)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
@@ -3887,7 +4166,7 @@
         <v>7</v>
       </c>
       <c r="E25">
-        <f>SUM(B25:D25)</f>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
     </row>
@@ -3905,7 +4184,7 @@
         <v>2</v>
       </c>
       <c r="E26">
-        <f>SUM(B26:D26)</f>
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
@@ -3923,7 +4202,7 @@
         <v>1</v>
       </c>
       <c r="E27">
-        <f>SUM(B27:D27)</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
     </row>
@@ -3941,7 +4220,7 @@
         <v>1</v>
       </c>
       <c r="E28">
-        <f>SUM(B28:D28)</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
     </row>
@@ -3959,7 +4238,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <f>SUM(B29:D29)</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
     </row>
@@ -3985,7 +4264,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926F0B60-E019-4C3D-8EAE-8F133A341416}">
   <dimension ref="A1:D29"/>
   <sheetViews>
@@ -3995,7 +4274,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" style="8" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4014,7 +4293,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B2">
@@ -4028,7 +4307,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3">
         <v>0</v>
       </c>
@@ -4040,7 +4319,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4">
         <v>0</v>
       </c>
@@ -4052,7 +4331,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5">
         <v>8</v>
       </c>
@@ -4064,7 +4343,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B6">
@@ -4078,7 +4357,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7">
         <v>62</v>
       </c>
@@ -4090,7 +4369,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8">
         <v>85</v>
       </c>
@@ -4102,7 +4381,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9">
         <v>33</v>
       </c>
@@ -4114,7 +4393,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="B10">
         <v>78</v>
       </c>
@@ -4126,7 +4405,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B11">
@@ -4140,7 +4419,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12">
         <v>78</v>
       </c>
@@ -4152,7 +4431,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13">
         <v>24</v>
       </c>
@@ -4164,7 +4443,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
+      <c r="A14" s="9"/>
       <c r="B14">
         <v>13</v>
       </c>
@@ -4176,7 +4455,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="3">
@@ -4190,7 +4469,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
+      <c r="A16" s="10"/>
       <c r="B16">
         <v>14</v>
       </c>
@@ -4202,7 +4481,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B17">
@@ -4216,7 +4495,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
+      <c r="A18" s="9"/>
       <c r="B18">
         <v>78</v>
       </c>
@@ -4228,7 +4507,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B19">
@@ -4316,7 +4595,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B26">
@@ -4330,7 +4609,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
+      <c r="A27" s="9"/>
       <c r="B27">
         <v>18</v>
       </c>
@@ -4342,7 +4621,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
+      <c r="A28" s="9"/>
       <c r="B28">
         <v>18</v>
       </c>
@@ -4354,7 +4633,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
+      <c r="A29" s="9"/>
       <c r="B29">
         <v>89</v>
       </c>
@@ -4380,17 +4659,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414F94CE-5509-43C5-947A-66CC62E64568}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.21875" style="10" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" style="8" customWidth="1"/>
     <col min="2" max="2" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4409,7 +4688,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B2">
@@ -4423,7 +4702,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3">
         <v>0</v>
       </c>
@@ -4435,7 +4714,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4">
         <v>0</v>
       </c>
@@ -4447,7 +4726,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5">
         <v>8</v>
       </c>
@@ -4459,7 +4738,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B6">
@@ -4473,7 +4752,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7">
         <v>62</v>
       </c>
@@ -4485,7 +4764,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B8">
@@ -4499,7 +4778,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B9">
@@ -4513,7 +4792,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B10">
@@ -4527,7 +4806,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="3">
         <v>62</v>
       </c>
@@ -4539,7 +4818,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12">
         <v>10</v>
       </c>
@@ -4551,7 +4830,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13">
         <v>3</v>
       </c>
@@ -4563,7 +4842,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
+      <c r="A14" s="9"/>
       <c r="B14">
         <v>18</v>
       </c>
@@ -4575,7 +4854,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
+      <c r="A15" s="9"/>
       <c r="B15">
         <v>18</v>
       </c>
@@ -4587,7 +4866,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
+      <c r="A16" s="9"/>
       <c r="B16">
         <v>89</v>
       </c>
@@ -4599,7 +4878,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
+      <c r="A17" s="9"/>
       <c r="B17">
         <v>71</v>
       </c>
@@ -4611,7 +4890,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
+      <c r="A18" s="9"/>
       <c r="B18">
         <v>78</v>
       </c>
@@ -4623,7 +4902,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
+      <c r="A19" s="9"/>
       <c r="B19">
         <v>12</v>
       </c>
@@ -4635,7 +4914,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
+      <c r="A20" s="9"/>
       <c r="B20">
         <v>52</v>
       </c>
@@ -4647,7 +4926,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
+      <c r="A21" s="9"/>
       <c r="B21">
         <v>39</v>
       </c>
@@ -4659,7 +4938,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
+      <c r="A22" s="9"/>
       <c r="B22">
         <v>24</v>
       </c>
@@ -4671,7 +4950,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
+      <c r="A23" s="9"/>
       <c r="B23">
         <v>13</v>
       </c>
@@ -4683,7 +4962,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B24">
@@ -4697,7 +4976,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
+      <c r="A25" s="9"/>
       <c r="B25">
         <v>33</v>
       </c>
@@ -4709,7 +4988,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
+      <c r="A26" s="9"/>
       <c r="B26">
         <v>78</v>
       </c>
@@ -4721,7 +5000,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
+      <c r="A27" s="9"/>
       <c r="B27">
         <v>40</v>
       </c>
@@ -4733,7 +5012,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
+      <c r="A28" s="9"/>
       <c r="B28">
         <v>47</v>
       </c>
@@ -4745,7 +5024,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
+      <c r="A29" s="9"/>
       <c r="B29">
         <v>32</v>
       </c>

</xml_diff>